<commit_message>
Web Scrapping Done 1
</commit_message>
<xml_diff>
--- a/Chennai_Colleges/ChennaiColleges.xlsx
+++ b/Chennai_Colleges/ChennaiColleges.xlsx
@@ -3,7 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Hindustan.xlsx" sheetId="1" r:id="rId1"/>
+    <sheet name="College.xlsx" sheetId="1" r:id="rId1"/>
+    <sheet name="VEL.xlsx" sheetId="2" r:id="rId2"/>
+    <sheet name="SSN.xlsx" sheetId="3" r:id="rId3"/>
+    <sheet name="IIT.xlsx" sheetId="4" r:id="rId4"/>
+    <sheet name="Hindustan.xlsx" sheetId="5" r:id="rId5"/>
+    <sheet name="Sathyabama.xlsx" sheetId="6" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
@@ -377,7 +382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -399,10 +404,205 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
+        <v>College of Engineering, Anna University - [CEG], Chennai</v>
+      </c>
+      <c r="B2" t="str">
+        <v>The College of Engineering, Guindy (CEG), is one of the top engineering colleges in the country and is affiliated to Anna University. It has been ranked at 9th position among the engineering colleges in India by NIRF 2019 Ranking. The college offers a range of B.Tech and M.Tech courses under various specializations. There are a total of 14 departments in the college. In addition to these courses, CEG also offers other PG Courses such as MBA, MCA, M.Sc, and Ph.D.The college provides state-of-the-art facilities like well-stocked libraries, laboratories with all technical equipment, computer center, and well-maintained hostels. The college offers 100% job placement in branded companies namely Microsoft, Qualcomm, Google, Amazon, and Caterpillar.</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>name</v>
+      </c>
+      <c r="B1" t="str">
+        <v>summary</v>
+      </c>
+      <c r="C1" t="str">
+        <v>courseName</v>
+      </c>
+      <c r="D1" t="str">
+        <v>fees</v>
+      </c>
+      <c r="E1" t="str">
+        <v>eligibility</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>VEL Tech, Chennai</v>
+      </c>
+      <c r="B2" t="str">
+        <v>VelTech, Chennai, established in 2009 is popular for offering B.Tech and B.Tech (Lateral) courses. It has been ranked 95th for B.Tech by NIRF 2020 and IndiaToday ranked the B.Tech course at 126th position in the year 2020. The varsity accepts VTUEEE and TNEA for admission to its B.Tech regular and lateral entry courses. Check VelTech Admission 2022The institute offers good placement opportunities, INR 10 LPA was the highest salary package offered to students in VelTech Placement 2020-21.</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>name</v>
+      </c>
+      <c r="B1" t="str">
+        <v>summary</v>
+      </c>
+      <c r="C1" t="str">
+        <v>courseName</v>
+      </c>
+      <c r="D1" t="str">
+        <v>fees</v>
+      </c>
+      <c r="E1" t="str">
+        <v>eligibility</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>SSN College of Engineering - [SSNCE], Chennai</v>
+      </c>
+      <c r="B2" t="str">
+        <v>SSN College of Engineering (SSNCE) is a private engineering college established in 1996 at Chennai, Tamil Nadu. It has been approved by AICTE and affiliated to Anna University. The college offers BE/B.Tech at the undergraduate level and ME/M.Tech at the postgraduate level. Applications for admissions are accepted online. The college has excellent academic and student-centric facilities. Almost 200+ companies visit the college and 95% of the students get recruited every year with an average salary of 5.61 lakhs.</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>name</v>
+      </c>
+      <c r="B1" t="str">
+        <v>summary</v>
+      </c>
+      <c r="C1" t="str">
+        <v>courseName</v>
+      </c>
+      <c r="D1" t="str">
+        <v>fees</v>
+      </c>
+      <c r="E1" t="str">
+        <v>eligibility</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>IIT Madras - Indian Institute of Technology - [IITM], Chennai</v>
+      </c>
+      <c r="B2" t="str">
+        <v>IIT Madras is recently ranked at #255 by the QS Global World Rankings 2022 whereas the QS Asia Rankings 2021 has ranked the institute at the 50th position. Over the years, IIT Madras has managed to maintain its 1st position rank in the NIRF Engineering Ranking with 89.93 scores. In the year 2021, IIT Madras is again ranked at 1 in the Engineering category by the NIRF 2021. Check IIT Madars Ranking 2021IITM has 16 academic departments and numerous research centers that offer postgraduate and undergraduate programs in distinct disciplines of Engineering, Technology, and Pure Sciences. The flagship program of IIT Madras is B.Tech CSE admission to which is strictly granted on the basis of the JEE Advanced entrance scores followed by the JoSAA Seat Allotment Process. In order to get admission in the B.Tech CSE Program at IIT Madras, a general category candidate is required to have scored a JEE Advanced rank of 158. However, the first-year fees for those taking admission into IIT Madras B.Tech is INR 75,116 while the average CTC at IIT Madras placement was INR 18.1 LPA, the highest CTC offered to a B.Tech student at IITM was INR 82.5 LPA. Check IIT Madras Placement 2021</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>name</v>
+      </c>
+      <c r="B1" t="str">
+        <v>summary</v>
+      </c>
+      <c r="C1" t="str">
+        <v>courseName</v>
+      </c>
+      <c r="D1" t="str">
+        <v>fees</v>
+      </c>
+      <c r="E1" t="str">
+        <v>eligibility</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
         <v>Hindustan Institute of Technology and Science - [HITS], Chennai</v>
       </c>
       <c r="B2" t="str">
         <v>Hindustan Institute of Technology and Science (HITS) in Chennai is recognized as a Deemed University under section 3 of the UGC Act 1956. Hindustan University offers various UG, Integrated, PG, Diploma, PG Diploma, M.Phil. and PhD courses in the fields of Engineering, Management, Science, Arts, and Commerce. Admission to these courses is on the basis of marks obtained in the Entrance Exam conducted by HITS, merits and other National level exams. The placements of the university range between 4-5 LPA with students placed in top reputed companies such as Accenture, Cognizant, Infosys, CSS Group, Amazo, etc. Check: HITS Chennai Admission 2022Here are some quick facts about Hindustan Institute of Technology and Sciences:</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>name</v>
+      </c>
+      <c r="B1" t="str">
+        <v>summary</v>
+      </c>
+      <c r="C1" t="str">
+        <v>courseName</v>
+      </c>
+      <c r="D1" t="str">
+        <v>fees</v>
+      </c>
+      <c r="E1" t="str">
+        <v>eligibility</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Sathyabama Institute of Science and Technology, Chennai</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Sathyabama Institute of Science and Technology, Chennai is a Christian Minority Institution established in 1987. It is a deemed-to-be University accredited with Grade ‘A’ by National Assessment and Accreditation Council (NAAC). Sathyabama Institute of Science and Technology offers various Undergraduate, Postgraduate and Doctoral Programs in the field of Engineering, Architecture, Dental, Arts, Commerce, and Science. Admission to these courses is done on the basis of the national level exams conducted all over the country.Sathyabama Institute of Science and Technology has begun registrations for B.E / B.Tech / B.Arch. / B.Des programs 2022-23 for admission through the institute-level entrance test, Sathyabama All-India Entrance Exam (SAEEE) 2022.</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Web Scrapping Done 2
</commit_message>
<xml_diff>
--- a/Chennai_Colleges/ChennaiColleges.xlsx
+++ b/Chennai_Colleges/ChennaiColleges.xlsx
@@ -6,9 +6,9 @@
     <sheet name="College.xlsx" sheetId="1" r:id="rId1"/>
     <sheet name="VEL.xlsx" sheetId="2" r:id="rId2"/>
     <sheet name="SSN.xlsx" sheetId="3" r:id="rId3"/>
-    <sheet name="IIT.xlsx" sheetId="4" r:id="rId4"/>
-    <sheet name="Hindustan.xlsx" sheetId="5" r:id="rId5"/>
-    <sheet name="Sathyabama.xlsx" sheetId="6" r:id="rId6"/>
+    <sheet name="Sathyabama.xlsx" sheetId="4" r:id="rId4"/>
+    <sheet name="IIT.xlsx" sheetId="5" r:id="rId5"/>
+    <sheet name="Hindustan.xlsx" sheetId="6" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
@@ -409,6 +409,15 @@
       <c r="B2" t="str">
         <v>The College of Engineering, Guindy (CEG), is one of the top engineering colleges in the country and is affiliated to Anna University. It has been ranked at 9th position among the engineering colleges in India by NIRF 2019 Ranking. The college offers a range of B.Tech and M.Tech courses under various specializations. There are a total of 14 departments in the college. In addition to these courses, CEG also offers other PG Courses such as MBA, MCA, M.Sc, and Ph.D.The college provides state-of-the-art facilities like well-stocked libraries, laboratories with all technical equipment, computer center, and well-maintained hostels. The college offers 100% job placement in branded companies namely Microsoft, Qualcomm, Google, Amazon, and Caterpillar.</v>
       </c>
+      <c r="C2" t="str">
+        <v/>
+      </c>
+      <c r="D2" t="str">
+        <v/>
+      </c>
+      <c r="E2" t="str">
+        <v/>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
@@ -448,6 +457,15 @@
       <c r="B2" t="str">
         <v>VelTech, Chennai, established in 2009 is popular for offering B.Tech and B.Tech (Lateral) courses. It has been ranked 95th for B.Tech by NIRF 2020 and IndiaToday ranked the B.Tech course at 126th position in the year 2020. The varsity accepts VTUEEE and TNEA for admission to its B.Tech regular and lateral entry courses. Check VelTech Admission 2022The institute offers good placement opportunities, INR 10 LPA was the highest salary package offered to students in VelTech Placement 2020-21.</v>
       </c>
+      <c r="C2" t="str">
+        <v/>
+      </c>
+      <c r="D2" t="str">
+        <v/>
+      </c>
+      <c r="E2" t="str">
+        <v/>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
@@ -487,6 +505,15 @@
       <c r="B2" t="str">
         <v>SSN College of Engineering (SSNCE) is a private engineering college established in 1996 at Chennai, Tamil Nadu. It has been approved by AICTE and affiliated to Anna University. The college offers BE/B.Tech at the undergraduate level and ME/M.Tech at the postgraduate level. Applications for admissions are accepted online. The college has excellent academic and student-centric facilities. Almost 200+ companies visit the college and 95% of the students get recruited every year with an average salary of 5.61 lakhs.</v>
       </c>
+      <c r="C2" t="str">
+        <v/>
+      </c>
+      <c r="D2" t="str">
+        <v/>
+      </c>
+      <c r="E2" t="str">
+        <v/>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
@@ -521,10 +548,19 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>IIT Madras - Indian Institute of Technology - [IITM], Chennai</v>
+        <v>Sathyabama Institute of Science and Technology, Chennai</v>
       </c>
       <c r="B2" t="str">
-        <v>IIT Madras is recently ranked at #255 by the QS Global World Rankings 2022 whereas the QS Asia Rankings 2021 has ranked the institute at the 50th position. Over the years, IIT Madras has managed to maintain its 1st position rank in the NIRF Engineering Ranking with 89.93 scores. In the year 2021, IIT Madras is again ranked at 1 in the Engineering category by the NIRF 2021. Check IIT Madars Ranking 2021IITM has 16 academic departments and numerous research centers that offer postgraduate and undergraduate programs in distinct disciplines of Engineering, Technology, and Pure Sciences. The flagship program of IIT Madras is B.Tech CSE admission to which is strictly granted on the basis of the JEE Advanced entrance scores followed by the JoSAA Seat Allotment Process. In order to get admission in the B.Tech CSE Program at IIT Madras, a general category candidate is required to have scored a JEE Advanced rank of 158. However, the first-year fees for those taking admission into IIT Madras B.Tech is INR 75,116 while the average CTC at IIT Madras placement was INR 18.1 LPA, the highest CTC offered to a B.Tech student at IITM was INR 82.5 LPA. Check IIT Madras Placement 2021</v>
+        <v>Sathyabama Institute of Science and Technology, Chennai is a Christian Minority Institution established in 1987. It is a deemed-to-be University accredited with Grade ‘A’ by National Assessment and Accreditation Council (NAAC). Sathyabama Institute of Science and Technology offers various Undergraduate, Postgraduate and Doctoral Programs in the field of Engineering, Architecture, Dental, Arts, Commerce, and Science. Admission to these courses is done on the basis of the national level exams conducted all over the country.Sathyabama Institute of Science and Technology has begun registrations for B.E / B.Tech / B.Arch. / B.Des programs 2022-23 for admission through the institute-level entrance test, Sathyabama All-India Entrance Exam (SAEEE) 2022.</v>
+      </c>
+      <c r="C2" t="str">
+        <v/>
+      </c>
+      <c r="D2" t="str">
+        <v/>
+      </c>
+      <c r="E2" t="str">
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -560,10 +596,19 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Hindustan Institute of Technology and Science - [HITS], Chennai</v>
+        <v>IIT Madras - Indian Institute of Technology - [IITM], Chennai</v>
       </c>
       <c r="B2" t="str">
-        <v>Hindustan Institute of Technology and Science (HITS) in Chennai is recognized as a Deemed University under section 3 of the UGC Act 1956. Hindustan University offers various UG, Integrated, PG, Diploma, PG Diploma, M.Phil. and PhD courses in the fields of Engineering, Management, Science, Arts, and Commerce. Admission to these courses is on the basis of marks obtained in the Entrance Exam conducted by HITS, merits and other National level exams. The placements of the university range between 4-5 LPA with students placed in top reputed companies such as Accenture, Cognizant, Infosys, CSS Group, Amazo, etc. Check: HITS Chennai Admission 2022Here are some quick facts about Hindustan Institute of Technology and Sciences:</v>
+        <v>IIT Madras is recently ranked at #255 by the QS Global World Rankings 2022 whereas the QS Asia Rankings 2021 has ranked the institute at the 50th position. Over the years, IIT Madras has managed to maintain its 1st position rank in the NIRF Engineering Ranking with 89.93 scores. In the year 2021, IIT Madras is again ranked at 1 in the Engineering category by the NIRF 2021. Check IIT Madars Ranking 2021IITM has 16 academic departments and numerous research centers that offer postgraduate and undergraduate programs in distinct disciplines of Engineering, Technology, and Pure Sciences. The flagship program of IIT Madras is B.Tech CSE admission to which is strictly granted on the basis of the JEE Advanced entrance scores followed by the JoSAA Seat Allotment Process. In order to get admission in the B.Tech CSE Program at IIT Madras, a general category candidate is required to have scored a JEE Advanced rank of 158. However, the first-year fees for those taking admission into IIT Madras B.Tech is INR 75,116 while the average CTC at IIT Madras placement was INR 18.1 LPA, the highest CTC offered to a B.Tech student at IITM was INR 82.5 LPA. Check IIT Madras Placement 2021</v>
+      </c>
+      <c r="C2" t="str">
+        <v/>
+      </c>
+      <c r="D2" t="str">
+        <v/>
+      </c>
+      <c r="E2" t="str">
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -599,10 +644,19 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Sathyabama Institute of Science and Technology, Chennai</v>
+        <v>Hindustan Institute of Technology and Science - [HITS], Chennai</v>
       </c>
       <c r="B2" t="str">
-        <v>Sathyabama Institute of Science and Technology, Chennai is a Christian Minority Institution established in 1987. It is a deemed-to-be University accredited with Grade ‘A’ by National Assessment and Accreditation Council (NAAC). Sathyabama Institute of Science and Technology offers various Undergraduate, Postgraduate and Doctoral Programs in the field of Engineering, Architecture, Dental, Arts, Commerce, and Science. Admission to these courses is done on the basis of the national level exams conducted all over the country.Sathyabama Institute of Science and Technology has begun registrations for B.E / B.Tech / B.Arch. / B.Des programs 2022-23 for admission through the institute-level entrance test, Sathyabama All-India Entrance Exam (SAEEE) 2022.</v>
+        <v>Hindustan Institute of Technology and Science (HITS) in Chennai is recognized as a Deemed University under section 3 of the UGC Act 1956. Hindustan University offers various UG, Integrated, PG, Diploma, PG Diploma, M.Phil. and PhD courses in the fields of Engineering, Management, Science, Arts, and Commerce. Admission to these courses is on the basis of marks obtained in the Entrance Exam conducted by HITS, merits and other National level exams. The placements of the university range between 4-5 LPA with students placed in top reputed companies such as Accenture, Cognizant, Infosys, CSS Group, Amazo, etc. Check: HITS Chennai Admission 2022Here are some quick facts about Hindustan Institute of Technology and Sciences:</v>
+      </c>
+      <c r="C2" t="str">
+        <v/>
+      </c>
+      <c r="D2" t="str">
+        <v/>
+      </c>
+      <c r="E2" t="str">
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Web Scrapping of Both Task is Done
</commit_message>
<xml_diff>
--- a/Chennai_Colleges/ChennaiColleges.xlsx
+++ b/Chennai_Colleges/ChennaiColleges.xlsx
@@ -4,11 +4,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="College.xlsx" sheetId="1" r:id="rId1"/>
-    <sheet name="VEL.xlsx" sheetId="2" r:id="rId2"/>
-    <sheet name="SSN.xlsx" sheetId="3" r:id="rId3"/>
-    <sheet name="Sathyabama.xlsx" sheetId="4" r:id="rId4"/>
-    <sheet name="IIT.xlsx" sheetId="5" r:id="rId5"/>
-    <sheet name="Hindustan.xlsx" sheetId="6" r:id="rId6"/>
+    <sheet name="IIT.xlsx" sheetId="2" r:id="rId2"/>
+    <sheet name="VEL.xlsx" sheetId="3" r:id="rId3"/>
+    <sheet name="Hindustan.xlsx" sheetId="4" r:id="rId4"/>
+    <sheet name="Sathyabama.xlsx" sheetId="5" r:id="rId5"/>
+    <sheet name="SSN.xlsx" sheetId="6" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
@@ -452,10 +452,10 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>VEL Tech, Chennai</v>
+        <v>IIT Madras - Indian Institute of Technology - [IITM], Chennai</v>
       </c>
       <c r="B2" t="str">
-        <v>VelTech, Chennai, established in 2009 is popular for offering B.Tech and B.Tech (Lateral) courses. It has been ranked 95th for B.Tech by NIRF 2020 and IndiaToday ranked the B.Tech course at 126th position in the year 2020. The varsity accepts VTUEEE and TNEA for admission to its B.Tech regular and lateral entry courses. Check VelTech Admission 2022The institute offers good placement opportunities, INR 10 LPA was the highest salary package offered to students in VelTech Placement 2020-21.</v>
+        <v>IIT Madras is recently ranked at #255 by the QS Global World Rankings 2022 whereas the QS Asia Rankings 2021 has ranked the institute at the 50th position. Over the years, IIT Madras has managed to maintain its 1st position rank in the NIRF Engineering Ranking with 89.93 scores. In the year 2021, IIT Madras is again ranked at 1 in the Engineering category by the NIRF 2021. Check IIT Madars Ranking 2021IITM has 16 academic departments and numerous research centers that offer postgraduate and undergraduate programs in distinct disciplines of Engineering, Technology, and Pure Sciences. The flagship program of IIT Madras is B.Tech CSE admission to which is strictly granted on the basis of the JEE Advanced entrance scores followed by the JoSAA Seat Allotment Process. In order to get admission in the B.Tech CSE Program at IIT Madras, a general category candidate is required to have scored a JEE Advanced rank of 158. However, the first-year fees for those taking admission into IIT Madras B.Tech is INR 75,116 while the average CTC at IIT Madras placement was INR 18.1 LPA, the highest CTC offered to a B.Tech student at IITM was INR 82.5 LPA. Check IIT Madras Placement 2021</v>
       </c>
       <c r="C2" t="str">
         <v/>
@@ -500,10 +500,10 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>SSN College of Engineering - [SSNCE], Chennai</v>
+        <v>VEL Tech, Chennai</v>
       </c>
       <c r="B2" t="str">
-        <v>SSN College of Engineering (SSNCE) is a private engineering college established in 1996 at Chennai, Tamil Nadu. It has been approved by AICTE and affiliated to Anna University. The college offers BE/B.Tech at the undergraduate level and ME/M.Tech at the postgraduate level. Applications for admissions are accepted online. The college has excellent academic and student-centric facilities. Almost 200+ companies visit the college and 95% of the students get recruited every year with an average salary of 5.61 lakhs.</v>
+        <v>VelTech, Chennai, established in 2009 is popular for offering B.Tech and B.Tech (Lateral) courses. It has been ranked 95th for B.Tech by NIRF 2020 and IndiaToday ranked the B.Tech course at 126th position in the year 2020. The varsity accepts VTUEEE and TNEA for admission to its B.Tech regular and lateral entry courses. Check VelTech Admission 2022The institute offers good placement opportunities, INR 10 LPA was the highest salary package offered to students in VelTech Placement 2020-21.</v>
       </c>
       <c r="C2" t="str">
         <v/>
@@ -548,10 +548,10 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Sathyabama Institute of Science and Technology, Chennai</v>
+        <v>Hindustan Institute of Technology and Science - [HITS], Chennai</v>
       </c>
       <c r="B2" t="str">
-        <v>Sathyabama Institute of Science and Technology, Chennai is a Christian Minority Institution established in 1987. It is a deemed-to-be University accredited with Grade ‘A’ by National Assessment and Accreditation Council (NAAC). Sathyabama Institute of Science and Technology offers various Undergraduate, Postgraduate and Doctoral Programs in the field of Engineering, Architecture, Dental, Arts, Commerce, and Science. Admission to these courses is done on the basis of the national level exams conducted all over the country.Sathyabama Institute of Science and Technology has begun registrations for B.E / B.Tech / B.Arch. / B.Des programs 2022-23 for admission through the institute-level entrance test, Sathyabama All-India Entrance Exam (SAEEE) 2022.</v>
+        <v>Hindustan Institute of Technology and Science (HITS) in Chennai is recognized as a Deemed University under section 3 of the UGC Act 1956. Hindustan University offers various UG, Integrated, PG, Diploma, PG Diploma, M.Phil. and PhD courses in the fields of Engineering, Management, Science, Arts, and Commerce. Admission to these courses is on the basis of marks obtained in the Entrance Exam conducted by HITS, merits and other National level exams. The placements of the university range between 4-5 LPA with students placed in top reputed companies such as Accenture, Cognizant, Infosys, CSS Group, Amazo, etc. Check: HITS Chennai Admission 2022Here are some quick facts about Hindustan Institute of Technology and Sciences:</v>
       </c>
       <c r="C2" t="str">
         <v/>
@@ -596,10 +596,10 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>IIT Madras - Indian Institute of Technology - [IITM], Chennai</v>
+        <v>Sathyabama Institute of Science and Technology, Chennai</v>
       </c>
       <c r="B2" t="str">
-        <v>IIT Madras is recently ranked at #255 by the QS Global World Rankings 2022 whereas the QS Asia Rankings 2021 has ranked the institute at the 50th position. Over the years, IIT Madras has managed to maintain its 1st position rank in the NIRF Engineering Ranking with 89.93 scores. In the year 2021, IIT Madras is again ranked at 1 in the Engineering category by the NIRF 2021. Check IIT Madars Ranking 2021IITM has 16 academic departments and numerous research centers that offer postgraduate and undergraduate programs in distinct disciplines of Engineering, Technology, and Pure Sciences. The flagship program of IIT Madras is B.Tech CSE admission to which is strictly granted on the basis of the JEE Advanced entrance scores followed by the JoSAA Seat Allotment Process. In order to get admission in the B.Tech CSE Program at IIT Madras, a general category candidate is required to have scored a JEE Advanced rank of 158. However, the first-year fees for those taking admission into IIT Madras B.Tech is INR 75,116 while the average CTC at IIT Madras placement was INR 18.1 LPA, the highest CTC offered to a B.Tech student at IITM was INR 82.5 LPA. Check IIT Madras Placement 2021</v>
+        <v>Sathyabama Institute of Science and Technology, Chennai is a Christian Minority Institution established in 1987. It is a deemed-to-be University accredited with Grade ‘A’ by National Assessment and Accreditation Council (NAAC). Sathyabama Institute of Science and Technology offers various Undergraduate, Postgraduate and Doctoral Programs in the field of Engineering, Architecture, Dental, Arts, Commerce, and Science. Admission to these courses is done on the basis of the national level exams conducted all over the country.Sathyabama Institute of Science and Technology has begun registrations for B.E / B.Tech / B.Arch. / B.Des programs 2022-23 for admission through the institute-level entrance test, Sathyabama All-India Entrance Exam (SAEEE) 2022.</v>
       </c>
       <c r="C2" t="str">
         <v/>
@@ -644,10 +644,10 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Hindustan Institute of Technology and Science - [HITS], Chennai</v>
+        <v>SSN College of Engineering - [SSNCE], Chennai</v>
       </c>
       <c r="B2" t="str">
-        <v>Hindustan Institute of Technology and Science (HITS) in Chennai is recognized as a Deemed University under section 3 of the UGC Act 1956. Hindustan University offers various UG, Integrated, PG, Diploma, PG Diploma, M.Phil. and PhD courses in the fields of Engineering, Management, Science, Arts, and Commerce. Admission to these courses is on the basis of marks obtained in the Entrance Exam conducted by HITS, merits and other National level exams. The placements of the university range between 4-5 LPA with students placed in top reputed companies such as Accenture, Cognizant, Infosys, CSS Group, Amazo, etc. Check: HITS Chennai Admission 2022Here are some quick facts about Hindustan Institute of Technology and Sciences:</v>
+        <v>SSN College of Engineering (SSNCE) is a private engineering college established in 1996 at Chennai, Tamil Nadu. It has been approved by AICTE and affiliated to Anna University. The college offers BE/B.Tech at the undergraduate level and ME/M.Tech at the postgraduate level. Applications for admissions are accepted online. The college has excellent academic and student-centric facilities. Almost 200+ companies visit the college and 95% of the students get recruited every year with an average salary of 5.61 lakhs.</v>
       </c>
       <c r="C2" t="str">
         <v/>

</xml_diff>